<commit_message>
CHUCHATV estimate pdf version
</commit_message>
<xml_diff>
--- a/Projects/CHUCHATV_Upgrades/Estimate.xlsx
+++ b/Projects/CHUCHATV_Upgrades/Estimate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lucasmac/Desktop/My_Projects.nosync/3D_Printer/FlyingBear-Gost-5/Projects/CHUCHATV_Upgrades/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{665A9D3F-8C39-E843-89CC-A2651ED74DAB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EBC0539-1595-EA42-9ED3-94CF4ED08628}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16180" tabRatio="754" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,32 +23,40 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="122">
+  <si>
+    <t xml:space="preserve">Vref </t>
+  </si>
+  <si>
+    <t>Irms</t>
+  </si>
+  <si>
+    <t>Imax</t>
+  </si>
   <si>
     <r>
       <rPr>
         <b/>
-        <sz val="11"/>
+        <sz val="10"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
+        <rFont val="Proxima_nova"/>
         <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Vref   -</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Напряжение  на  драйвере</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Vref </t>
+      </rPr>
+      <t>Vref</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF444444"/>
+        <rFont val="Proxima_nova"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> = (Irms * 2.5) / 1.77</t>
+    </r>
+  </si>
+  <si>
+    <t>Vref</t>
   </si>
   <si>
     <r>
@@ -63,35 +71,17 @@
     </r>
     <r>
       <rPr>
+        <b/>
         <sz val="10"/>
         <color rgb="FF444444"/>
         <rFont val="Proxima_nova"/>
         <charset val="134"/>
       </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF444444"/>
-        <rFont val="Proxima_nova"/>
-        <charset val="204"/>
-      </rPr>
-      <t xml:space="preserve">- </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF444444"/>
-        <rFont val="Proxima_nova"/>
-        <charset val="134"/>
-      </rPr>
-      <t>Постоянный ток на двигателях.</t>
-    </r>
-  </si>
-  <si>
-    <t>Irms</t>
+      <t xml:space="preserve"> = (Vref * 1.77) / 2.5</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Irms </t>
   </si>
   <si>
     <r>
@@ -110,53 +100,21 @@
         <sz val="10"/>
         <color rgb="FF444444"/>
         <rFont val="Proxima_nova"/>
-        <charset val="204"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> = Irms * 1.41</t>
+    </r>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
         <sz val="10"/>
-        <color theme="9" tint="-0.249977111117893"/>
+        <color theme="3" tint="-0.249977111117893"/>
         <rFont val="Proxima_nova"/>
         <charset val="204"/>
       </rPr>
-      <t>-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF444444"/>
-        <rFont val="Proxima_nova"/>
-        <charset val="204"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF444444"/>
-        <rFont val="Proxima_nova"/>
-        <charset val="134"/>
-      </rPr>
-      <t>Пиковый ток  на двигателях</t>
-    </r>
-  </si>
-  <si>
-    <t>Imax</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Proxima_nova"/>
-        <charset val="204"/>
-      </rPr>
-      <t>Vref</t>
+      <t>Irms</t>
     </r>
     <r>
       <rPr>
@@ -166,123 +124,7 @@
         <rFont val="Proxima_nova"/>
         <charset val="134"/>
       </rPr>
-      <t xml:space="preserve"> = (Irms * 2.5) / 1.77</t>
-    </r>
-  </si>
-  <si>
-    <t>Vref</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="3" tint="-0.249977111117893"/>
-        <rFont val="Proxima_nova"/>
-        <charset val="204"/>
-      </rPr>
-      <t>Irms</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF444444"/>
-        <rFont val="Proxima_nova"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve"> = (Vref * 1.77) / 2.5</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Irms </t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="9" tint="-0.249977111117893"/>
-        <rFont val="Proxima_nova"/>
-        <charset val="204"/>
-      </rPr>
-      <t>Imax</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF444444"/>
-        <rFont val="Proxima_nova"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve"> = Irms * 1.41</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="3" tint="-0.249977111117893"/>
-        <rFont val="Proxima_nova"/>
-        <charset val="204"/>
-      </rPr>
-      <t>Irms</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF444444"/>
-        <rFont val="Proxima_nova"/>
-        <charset val="134"/>
-      </rPr>
       <t xml:space="preserve"> = Imax / 1.41</t>
-    </r>
-  </si>
-  <si>
-    <t>Параметры</t>
-  </si>
-  <si>
-    <t>известно</t>
-  </si>
-  <si>
-    <t>нужно узнать</t>
-  </si>
-  <si>
-    <t>формула</t>
-  </si>
-  <si>
-    <t>какие  значения  ставить</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <charset val="204"/>
-      </rPr>
-      <t>Начальная  скорость (Jerk) V</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <charset val="204"/>
-      </rPr>
-      <t>0</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <charset val="204"/>
-      </rPr>
-      <t>, мм/с</t>
     </r>
   </si>
   <si>
@@ -327,9 +169,6 @@
     <t>t</t>
   </si>
   <si>
-    <t>Конечная  скорость(скорость печати)  V, мм/с</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -367,27 +206,6 @@
   <si>
     <r>
       <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <charset val="204"/>
-      </rPr>
-      <t>Ускорение (ACCELERATION) а, мм/с</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="204"/>
-      </rPr>
-      <t>²</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
         <b/>
         <sz val="11"/>
         <color theme="1"/>
@@ -421,9 +239,6 @@
     <t>S</t>
   </si>
   <si>
-    <t>Время  t,с</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -456,9 +271,6 @@
     </r>
   </si>
   <si>
-    <t>Перемещение   S, мм</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -491,63 +303,6 @@
     </r>
   </si>
   <si>
-    <t>Jerk вводим  значения</t>
-  </si>
-  <si>
-    <t>ACCELERATION вводим  значения</t>
-  </si>
-  <si>
-    <t>d- JUNCTION_DEVIATION РЕЗУЛЬТАТ</t>
-  </si>
-  <si>
-    <t>M302 P1 ; Отключение температурной защиты экструденра</t>
-  </si>
-  <si>
-    <t>G92 E0 ; Сброс позиции экструдера</t>
-  </si>
-  <si>
-    <t>Для начала настройки шагов нам необходимо освободить филамент из принтера. Для этого необходимо нагреть сопло до рабочей температуры (проще всего это сделать запустив преднагрев экструдера на принтере), дальше немного(3-5 мм) выдавить филамент в сторону стола, после чего откатить его назад на 7-8 см. После этой операции можно смело вытаскивать филамент руками не боясь ничего повредить.</t>
-  </si>
-  <si>
-    <t>1. Вытаскиваем ptfe-трубку из фитинга фидера. Для этого нажимаем на черное кольцо на фитинге по мере возможностей равномерно и до упора, в этом положении фитинг отпускает трубку и она вытаскивается без приложения силы.</t>
-  </si>
-  <si>
-    <t>2. Чутка отматываем пластик назад на катушку, из фидера должен выходить ровный(не оплавленный) филамент. Отрезаем его ровно по краю фитинга.</t>
-  </si>
-  <si>
-    <t>3. Заходим в куру, подключаемся к принтеру по WiFi, переходим на вкладку монитор и в окно Send g-code по очереди отправляем следующие строчки</t>
-  </si>
-  <si>
-    <t>Длину выдавливаемого пластика лучше подобрать исходя из размеров имеющейся у вас линейки, выдавливайте на 10% меньше.</t>
-  </si>
-  <si>
-    <t>4. Отрезаем выдвинутый пластик точно так же по краю фитинга. Измеряем длину отрезанного куска - для примера 265 мм.</t>
-  </si>
-  <si>
-    <t>400*280/265=422.64</t>
-  </si>
-  <si>
-    <t>6. Берём из прошивки файл robin_nano35_cfg.txt находим в нём параметр &gt;DEFAULT_E0_STEPS_PER_UNIT и заменяем его значение на полученное в прошлом шаге. Сохраняем, кладём файл в корень sd карты и перезагружаем принтер.</t>
-  </si>
-  <si>
-    <t>7. Рекомендуется повторить процедуру начиная с шага 3.</t>
-  </si>
-  <si>
-    <t>8. Собираем назад принтер.</t>
-  </si>
-  <si>
-    <t>- Узнаем текущее кол-во шагов на мм, (команда M503)</t>
-  </si>
-  <si>
-    <t>- Вноситм в прошивку, или побыстрому в память: M92 E***</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Умножаем на полученный коэфф.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Не забываем сохранить M500.</t>
-  </si>
-  <si>
     <t>ссылка на  товар</t>
   </si>
   <si>
@@ -740,13 +495,7 @@
     <t>d- JUNCTION_DEVIATION RESULT</t>
   </si>
   <si>
-    <t>G1 E280 F800 ; Выдавить 280 мм пластика</t>
-  </si>
-  <si>
     <t>G1 E280 F800; Extrude 280mm plastic</t>
-  </si>
-  <si>
-    <t>5. Высчитываем правильное количество шагов мотора на мм. Для этого берём текущее значение шагов в ПРОШИВКЕ (по умолчанию 400) умножаем на длину которую запрашивали выдавить (в примере 280) и делим на полученный результат (в примере 265):</t>
   </si>
   <si>
     <t>5. Calculate the correct number of motor steps per mm. To do this, we take the current value of the steps (IN THE FIRMWARE by default 400), multiply by the length that was requested to extrude (in example 280) and divide by the result obtained (in example 265):</t>
@@ -911,12 +660,126 @@
   <si>
     <t>8x22x7 mm 608ZZ</t>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Vref   -</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Driver voltage</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="3" tint="-0.249977111117893"/>
+        <rFont val="Proxima_nova"/>
+        <charset val="204"/>
+      </rPr>
+      <t>Irms</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF444444"/>
+        <rFont val="Proxima_nova"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF444444"/>
+        <rFont val="Proxima_nova"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">- </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF444444"/>
+        <rFont val="Proxima_nova"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Constant current on motors.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Proxima_nova"/>
+        <charset val="204"/>
+      </rPr>
+      <t>Imax</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF444444"/>
+        <rFont val="Proxima_nova"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Proxima_nova"/>
+        <charset val="204"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF444444"/>
+        <rFont val="Proxima_nova"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF444444"/>
+        <rFont val="Proxima_nova"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Peak current on motors</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="26">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1003,19 +866,6 @@
       <name val="Calibri"/>
       <charset val="204"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="204"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="204"/>
     </font>
     <font>
       <b/>
@@ -1442,7 +1292,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
@@ -1611,7 +1461,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
@@ -1624,13 +1474,13 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="21" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="21" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1654,25 +1504,25 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1684,7 +1534,7 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2261,57 +2111,11 @@
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>154677</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>85311</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>79389</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>364435</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4551045" y="3369310"/>
-          <a:ext cx="1616710" cy="1132205"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>154677</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>85311</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1572952" cy="1123950"/>
@@ -2638,7 +2442,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
@@ -2658,34 +2462,34 @@
     <row r="1" spans="1:10" ht="39.75" customHeight="1" thickBot="1">
       <c r="A1" s="54"/>
       <c r="B1" s="54" t="s">
-        <v>144</v>
+        <v>110</v>
       </c>
       <c r="C1" s="56" t="s">
-        <v>148</v>
+        <v>114</v>
       </c>
       <c r="D1" s="55" t="s">
-        <v>140</v>
+        <v>106</v>
       </c>
       <c r="E1" s="56" t="s">
-        <v>141</v>
+        <v>107</v>
       </c>
       <c r="F1" s="55" t="s">
-        <v>142</v>
+        <v>108</v>
       </c>
       <c r="G1" s="57" t="s">
-        <v>143</v>
+        <v>109</v>
       </c>
       <c r="H1" s="58" t="s">
-        <v>51</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="18">
       <c r="A2" s="63"/>
       <c r="B2" s="63" t="s">
-        <v>70</v>
+        <v>38</v>
       </c>
       <c r="C2" s="64" t="s">
-        <v>83</v>
+        <v>51</v>
       </c>
       <c r="D2" s="64">
         <v>1</v>
@@ -2701,16 +2505,16 @@
         <v>5.9</v>
       </c>
       <c r="H2" s="66" t="s">
-        <v>52</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="18">
       <c r="A3" s="59"/>
       <c r="B3" s="59" t="s">
-        <v>71</v>
+        <v>39</v>
       </c>
       <c r="C3" s="60" t="s">
-        <v>54</v>
+        <v>22</v>
       </c>
       <c r="D3" s="60">
         <v>1</v>
@@ -2726,16 +2530,16 @@
         <v>1.17</v>
       </c>
       <c r="H3" s="61" t="s">
-        <v>53</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="18">
       <c r="A4" s="59"/>
       <c r="B4" s="59" t="s">
-        <v>72</v>
+        <v>40</v>
       </c>
       <c r="C4" s="60" t="s">
-        <v>56</v>
+        <v>24</v>
       </c>
       <c r="D4" s="60">
         <v>1</v>
@@ -2751,16 +2555,16 @@
         <v>0.5</v>
       </c>
       <c r="H4" s="61" t="s">
-        <v>55</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="18">
       <c r="A5" s="59"/>
       <c r="B5" s="59" t="s">
-        <v>73</v>
+        <v>41</v>
       </c>
       <c r="C5" s="60" t="s">
-        <v>84</v>
+        <v>52</v>
       </c>
       <c r="D5" s="60">
         <v>1</v>
@@ -2776,13 +2580,13 @@
         <v>2.5199999999999996</v>
       </c>
       <c r="H5" s="61" t="s">
-        <v>57</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="18">
       <c r="A6" s="59"/>
       <c r="B6" s="59" t="s">
-        <v>74</v>
+        <v>42</v>
       </c>
       <c r="C6" s="60"/>
       <c r="D6" s="60">
@@ -2799,16 +2603,16 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="H6" s="61" t="s">
-        <v>58</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="18">
       <c r="A7" s="73"/>
       <c r="B7" s="73" t="s">
-        <v>124</v>
+        <v>90</v>
       </c>
       <c r="C7" s="60" t="s">
-        <v>60</v>
+        <v>28</v>
       </c>
       <c r="D7" s="60">
         <v>2</v>
@@ -2824,16 +2628,16 @@
         <v>3.42</v>
       </c>
       <c r="H7" s="61" t="s">
-        <v>59</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="17">
       <c r="A8" s="73"/>
       <c r="B8" s="73" t="s">
-        <v>123</v>
+        <v>89</v>
       </c>
       <c r="C8" s="74" t="s">
-        <v>122</v>
+        <v>88</v>
       </c>
       <c r="D8" s="60">
         <v>1</v>
@@ -2849,13 +2653,13 @@
         <v>1</v>
       </c>
       <c r="H8" s="68" t="s">
-        <v>121</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="18">
       <c r="A9" s="59"/>
       <c r="B9" s="59" t="s">
-        <v>75</v>
+        <v>43</v>
       </c>
       <c r="C9" s="60"/>
       <c r="D9" s="60">
@@ -2872,16 +2676,16 @@
         <v>10.38</v>
       </c>
       <c r="H9" s="61" t="s">
-        <v>61</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="17">
       <c r="A10" s="62"/>
       <c r="B10" s="62" t="s">
-        <v>77</v>
+        <v>45</v>
       </c>
       <c r="C10" s="69" t="s">
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="D10" s="69">
         <v>1</v>
@@ -2897,7 +2701,7 @@
         <v>3.82</v>
       </c>
       <c r="H10" s="68" t="s">
-        <v>63</v>
+        <v>31</v>
       </c>
       <c r="I10" s="21"/>
       <c r="J10" s="21"/>
@@ -2905,7 +2709,7 @@
     <row r="11" spans="1:10" ht="17">
       <c r="A11" s="62"/>
       <c r="B11" s="62" t="s">
-        <v>78</v>
+        <v>46</v>
       </c>
       <c r="C11" s="69"/>
       <c r="D11" s="69">
@@ -2922,7 +2726,7 @@
         <v>3</v>
       </c>
       <c r="H11" s="68" t="s">
-        <v>65</v>
+        <v>33</v>
       </c>
       <c r="I11" s="21"/>
       <c r="J11" s="21"/>
@@ -2930,7 +2734,7 @@
     <row r="12" spans="1:10" ht="17">
       <c r="A12" s="72"/>
       <c r="B12" s="62" t="s">
-        <v>79</v>
+        <v>47</v>
       </c>
       <c r="C12" s="69"/>
       <c r="D12" s="69">
@@ -2947,7 +2751,7 @@
         <v>2.02</v>
       </c>
       <c r="H12" s="68" t="s">
-        <v>66</v>
+        <v>34</v>
       </c>
       <c r="I12" s="21"/>
       <c r="J12" s="21"/>
@@ -2955,10 +2759,10 @@
     <row r="13" spans="1:10" ht="17">
       <c r="A13" s="62"/>
       <c r="B13" s="62" t="s">
-        <v>80</v>
+        <v>48</v>
       </c>
       <c r="C13" s="75" t="s">
-        <v>68</v>
+        <v>36</v>
       </c>
       <c r="D13" s="69">
         <v>1</v>
@@ -2974,7 +2778,7 @@
         <v>7.6</v>
       </c>
       <c r="H13" s="68" t="s">
-        <v>67</v>
+        <v>35</v>
       </c>
       <c r="I13" s="21"/>
       <c r="J13" s="21"/>
@@ -2982,10 +2786,10 @@
     <row r="14" spans="1:10" ht="17">
       <c r="A14" s="72"/>
       <c r="B14" s="72" t="s">
-        <v>125</v>
+        <v>91</v>
       </c>
       <c r="C14" s="75" t="s">
-        <v>149</v>
+        <v>115</v>
       </c>
       <c r="D14" s="69">
         <v>2</v>
@@ -3001,7 +2805,7 @@
         <v>4</v>
       </c>
       <c r="H14" s="68" t="s">
-        <v>119</v>
+        <v>85</v>
       </c>
       <c r="I14" s="21"/>
       <c r="J14" s="21"/>
@@ -3009,10 +2813,10 @@
     <row r="15" spans="1:10" ht="17">
       <c r="A15" s="62"/>
       <c r="B15" s="62" t="s">
-        <v>81</v>
+        <v>49</v>
       </c>
       <c r="C15" s="69" t="s">
-        <v>150</v>
+        <v>116</v>
       </c>
       <c r="D15" s="69"/>
       <c r="E15" s="69"/>
@@ -3028,10 +2832,10 @@
     <row r="16" spans="1:10" ht="17">
       <c r="A16" s="62"/>
       <c r="B16" s="62" t="s">
-        <v>82</v>
+        <v>50</v>
       </c>
       <c r="C16" s="69" t="s">
-        <v>151</v>
+        <v>117</v>
       </c>
       <c r="D16" s="69"/>
       <c r="E16" s="69"/>
@@ -3047,10 +2851,10 @@
     <row r="17" spans="1:11" ht="17">
       <c r="A17" s="62"/>
       <c r="B17" s="62" t="s">
-        <v>82</v>
+        <v>50</v>
       </c>
       <c r="C17" s="69" t="s">
-        <v>151</v>
+        <v>117</v>
       </c>
       <c r="D17" s="69"/>
       <c r="E17" s="69"/>
@@ -3066,10 +2870,10 @@
     <row r="18" spans="1:11" ht="17">
       <c r="A18" s="72"/>
       <c r="B18" s="72" t="s">
-        <v>139</v>
+        <v>105</v>
       </c>
       <c r="C18" s="75" t="s">
-        <v>152</v>
+        <v>118</v>
       </c>
       <c r="D18" s="69">
         <v>10</v>
@@ -3085,10 +2889,10 @@
         <v>4</v>
       </c>
       <c r="H18" s="68" t="s">
-        <v>138</v>
+        <v>104</v>
       </c>
       <c r="I18" s="82" t="s">
-        <v>145</v>
+        <v>111</v>
       </c>
       <c r="J18" s="83"/>
       <c r="K18" s="83"/>
@@ -3110,7 +2914,7 @@
     </row>
     <row r="21" spans="1:11" ht="27" thickBot="1">
       <c r="A21" s="79" t="s">
-        <v>146</v>
+        <v>112</v>
       </c>
       <c r="B21" s="80"/>
       <c r="C21" s="80"/>
@@ -3123,7 +2927,7 @@
     <row r="22" spans="1:11" ht="17">
       <c r="A22" s="62"/>
       <c r="B22" s="62" t="s">
-        <v>76</v>
+        <v>44</v>
       </c>
       <c r="C22" s="69"/>
       <c r="D22" s="69">
@@ -3140,7 +2944,7 @@
         <v>13</v>
       </c>
       <c r="H22" s="68" t="s">
-        <v>62</v>
+        <v>30</v>
       </c>
       <c r="I22" s="21"/>
       <c r="J22" s="21"/>
@@ -3148,7 +2952,7 @@
     <row r="23" spans="1:11" ht="17">
       <c r="A23" s="72"/>
       <c r="B23" s="72" t="s">
-        <v>126</v>
+        <v>92</v>
       </c>
       <c r="C23" s="69"/>
       <c r="D23" s="69">
@@ -3165,7 +2969,7 @@
         <v>2</v>
       </c>
       <c r="H23" s="68" t="s">
-        <v>120</v>
+        <v>86</v>
       </c>
       <c r="I23" s="21"/>
       <c r="J23" s="21"/>
@@ -3173,10 +2977,10 @@
     <row r="24" spans="1:11" ht="17">
       <c r="A24" s="72"/>
       <c r="B24" s="72" t="s">
-        <v>128</v>
+        <v>94</v>
       </c>
       <c r="C24" s="75" t="s">
-        <v>129</v>
+        <v>95</v>
       </c>
       <c r="D24" s="69">
         <v>1</v>
@@ -3192,10 +2996,10 @@
         <v>9</v>
       </c>
       <c r="H24" s="68" t="s">
-        <v>127</v>
+        <v>93</v>
       </c>
       <c r="I24" s="82" t="s">
-        <v>145</v>
+        <v>111</v>
       </c>
       <c r="J24" s="83"/>
       <c r="K24" s="83"/>
@@ -3208,7 +3012,7 @@
     </row>
     <row r="27" spans="1:11" ht="27" thickBot="1">
       <c r="A27" s="84" t="s">
-        <v>147</v>
+        <v>113</v>
       </c>
       <c r="B27" s="80"/>
       <c r="C27" s="80"/>
@@ -3221,10 +3025,10 @@
     <row r="28" spans="1:11" ht="17">
       <c r="A28" s="72"/>
       <c r="B28" s="72" t="s">
-        <v>130</v>
+        <v>96</v>
       </c>
       <c r="C28" s="75" t="s">
-        <v>135</v>
+        <v>101</v>
       </c>
       <c r="D28" s="69">
         <v>1</v>
@@ -3240,7 +3044,7 @@
         <v>44</v>
       </c>
       <c r="H28" s="68" t="s">
-        <v>131</v>
+        <v>97</v>
       </c>
       <c r="I28" s="21"/>
       <c r="J28" s="21"/>
@@ -3248,10 +3052,10 @@
     <row r="29" spans="1:11" ht="17">
       <c r="A29" s="72"/>
       <c r="B29" s="72" t="s">
-        <v>133</v>
+        <v>99</v>
       </c>
       <c r="C29" s="75" t="s">
-        <v>134</v>
+        <v>100</v>
       </c>
       <c r="D29" s="69">
         <v>1</v>
@@ -3267,7 +3071,7 @@
         <v>1.2</v>
       </c>
       <c r="H29" s="68" t="s">
-        <v>132</v>
+        <v>98</v>
       </c>
       <c r="I29" s="21"/>
       <c r="J29" s="21"/>
@@ -3275,7 +3079,7 @@
     <row r="30" spans="1:11" ht="17">
       <c r="A30" s="72"/>
       <c r="B30" s="72" t="s">
-        <v>136</v>
+        <v>102</v>
       </c>
       <c r="C30" s="75"/>
       <c r="D30" s="69">
@@ -3292,7 +3096,7 @@
         <v>8</v>
       </c>
       <c r="H30" s="68" t="s">
-        <v>137</v>
+        <v>103</v>
       </c>
       <c r="I30" s="82"/>
       <c r="J30" s="83"/>
@@ -3512,7 +3316,7 @@
     <hyperlink ref="H18" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId21"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId21"/>
   <drawing r:id="rId22"/>
 </worksheet>
 </file>
@@ -3522,7 +3326,7 @@
   <dimension ref="A2:L9"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
@@ -3538,14 +3342,14 @@
   <sheetData>
     <row r="2" spans="1:7">
       <c r="A2" s="35" t="s">
+        <v>119</v>
+      </c>
+      <c r="B2" s="36" t="s">
         <v>0</v>
-      </c>
-      <c r="B2" s="36" t="s">
-        <v>1</v>
       </c>
       <c r="C2" s="37"/>
       <c r="D2" s="67" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
       <c r="E2" s="67"/>
       <c r="F2" s="67"/>
@@ -3553,14 +3357,14 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="38" t="s">
-        <v>2</v>
+        <v>120</v>
       </c>
       <c r="B3" s="39" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C3" s="37"/>
       <c r="D3" s="67" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
       <c r="E3" s="67"/>
       <c r="F3" s="67"/>
@@ -3568,14 +3372,14 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="40" t="s">
-        <v>4</v>
+        <v>121</v>
       </c>
       <c r="B4" s="41" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C4" s="42"/>
       <c r="D4" s="67" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
       <c r="E4" s="67"/>
       <c r="F4" s="67"/>
@@ -3586,10 +3390,10 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="44" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B6" s="45" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C6" s="46">
         <f>(C3*2.5)/1.77</f>
@@ -3598,10 +3402,10 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="47" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B7" s="48" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C7" s="49">
         <f>(C2*1.77)/2.5</f>
@@ -3610,10 +3414,10 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="47" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B8" s="50" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C8" s="49">
         <f>C3*1.41</f>
@@ -3622,10 +3426,10 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="51" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B9" s="52" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C9" s="53">
         <f>C4/1.41</f>
@@ -3634,15 +3438,16 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -3655,356 +3460,192 @@
     <col min="8" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="31.25" customHeight="1">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:7" ht="33.5" customHeight="1">
+      <c r="A1" s="70"/>
+      <c r="B1" s="70"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="71"/>
+    </row>
+    <row r="2" spans="1:7" ht="54.75" customHeight="1" thickBot="1">
+      <c r="A2" s="88" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="88"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="88"/>
+    </row>
+    <row r="3" spans="1:7" ht="31.25" customHeight="1" thickBot="1">
+      <c r="A3" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="E3" s="85" t="s">
+        <v>79</v>
+      </c>
+      <c r="F3" s="86"/>
+      <c r="G3" s="87"/>
+    </row>
+    <row r="4" spans="1:7" ht="36.5" customHeight="1" thickBot="1">
+      <c r="A4" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="8">
+        <f>B5-(B6*B7)</f>
+        <v>0</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="3" t="s">
+    </row>
+    <row r="5" spans="1:7" ht="36.5" customHeight="1" thickBot="1">
+      <c r="A5" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="8">
+        <f>B4+(B6*B7)</f>
+        <v>0</v>
+      </c>
+      <c r="D5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="E5" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E1" s="85" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="86"/>
-      <c r="G1" s="87"/>
-    </row>
-    <row r="2" spans="1:7" ht="36.5" customHeight="1">
-      <c r="A2" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="8">
-        <f>B3-(B4*B5)</f>
-        <v>0</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" s="12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="36.5" customHeight="1">
-      <c r="A3" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="8">
-        <f>B2+(B4*B5)</f>
-        <v>0</v>
-      </c>
-      <c r="D3" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="F3" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" s="12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="36.5" customHeight="1">
-      <c r="A4" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="8" t="e">
-        <f>((B3*B3)-(B2*B2))/(2*B6)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D4" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="G4" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="36.5" customHeight="1">
-      <c r="A5" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="8" t="e">
-        <f>(B3-B2)/B4</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>19</v>
-      </c>
       <c r="F5" s="11" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="36.5" customHeight="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="36.5" customHeight="1" thickBot="1">
       <c r="A6" s="6" t="s">
-        <v>30</v>
+        <v>72</v>
       </c>
       <c r="B6" s="7"/>
       <c r="C6" s="8" t="e">
-        <f>((B3*B3)-(B2*B2))/(2*B4)</f>
+        <f>((B5*B5)-(B4*B4))/(2*B8)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D6" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" s="18" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="16.5" customHeight="1"/>
-    <row r="8" spans="1:7" ht="33.5" customHeight="1">
-      <c r="A8" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="B8" s="20"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="23"/>
-    </row>
-    <row r="9" spans="1:7" ht="33.5" customHeight="1">
-      <c r="A9" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="B9" s="25"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="28"/>
-    </row>
+      <c r="D6" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="36.5" customHeight="1" thickBot="1">
+      <c r="A7" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B7" s="7"/>
+      <c r="C7" s="8" t="e">
+        <f>(B5-B4)/B6</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="36.5" customHeight="1" thickBot="1">
+      <c r="A8" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="8" t="e">
+        <f>((B5*B5)-(B4*B4))/(2*B6)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="21.75" customHeight="1" thickBot="1"/>
     <row r="10" spans="1:7" ht="33.5" customHeight="1" thickBot="1">
-      <c r="A10" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="B10" s="30" t="e">
-        <f>(0.4*(B8*B8))/B9</f>
+      <c r="A10" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="B10" s="20"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="23"/>
+    </row>
+    <row r="11" spans="1:7" ht="33.5" customHeight="1" thickBot="1">
+      <c r="A11" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="B11" s="25"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="28"/>
+    </row>
+    <row r="12" spans="1:7" ht="33.5" customHeight="1" thickBot="1">
+      <c r="A12" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="B12" s="30" t="e">
+        <f>(0.4*(B10*B10))/B11</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="C10" s="21"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="32"/>
-      <c r="F10" s="33"/>
-    </row>
-    <row r="11" spans="1:7" ht="33.5" customHeight="1">
-      <c r="A11" s="70"/>
-      <c r="B11" s="70"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="27"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="71"/>
-    </row>
-    <row r="12" spans="1:7" ht="54.75" customHeight="1" thickBot="1">
-      <c r="A12" s="88" t="s">
-        <v>69</v>
-      </c>
-      <c r="B12" s="88"/>
-      <c r="C12" s="88"/>
-      <c r="D12" s="88"/>
-      <c r="E12" s="88"/>
-      <c r="F12" s="88"/>
-      <c r="G12" s="88"/>
-    </row>
-    <row r="13" spans="1:7" ht="31.25" customHeight="1" thickBot="1">
-      <c r="A13" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="E13" s="85" t="s">
-        <v>111</v>
-      </c>
-      <c r="F13" s="86"/>
-      <c r="G13" s="87"/>
-    </row>
-    <row r="14" spans="1:7" ht="36.5" customHeight="1" thickBot="1">
-      <c r="A14" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="B14" s="7"/>
-      <c r="C14" s="8">
-        <f>B15-(B16*B17)</f>
-        <v>0</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="F14" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="G14" s="12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="36.5" customHeight="1" thickBot="1">
-      <c r="A15" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="8">
-        <f>B14+(B16*B17)</f>
-        <v>0</v>
-      </c>
-      <c r="D15" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="F15" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="G15" s="12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="36.5" customHeight="1" thickBot="1">
-      <c r="A16" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="B16" s="7"/>
-      <c r="C16" s="8" t="e">
-        <f>((B15*B15)-(B14*B14))/(2*B18)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D16" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="E16" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="F16" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="G16" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="36.5" customHeight="1" thickBot="1">
-      <c r="A17" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="B17" s="7"/>
-      <c r="C17" s="8" t="e">
-        <f>(B15-B14)/B16</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D17" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="E17" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="F17" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="G17" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="36.5" customHeight="1" thickBot="1">
-      <c r="A18" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="B18" s="7"/>
-      <c r="C18" s="8" t="e">
-        <f>((B15*B15)-(B14*B14))/(2*B16)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D18" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="E18" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="F18" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="G18" s="18" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="21.75" customHeight="1" thickBot="1"/>
-    <row r="20" spans="1:7" ht="33.5" customHeight="1" thickBot="1">
-      <c r="A20" s="19" t="s">
-        <v>112</v>
-      </c>
-      <c r="B20" s="20"/>
-      <c r="C20" s="21"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="22"/>
-      <c r="F20" s="23"/>
-    </row>
-    <row r="21" spans="1:7" ht="33.5" customHeight="1" thickBot="1">
-      <c r="A21" s="24" t="s">
-        <v>113</v>
-      </c>
-      <c r="B21" s="25"/>
-      <c r="C21" s="21"/>
-      <c r="D21" s="26"/>
-      <c r="E21" s="27"/>
-      <c r="F21" s="28"/>
-    </row>
-    <row r="22" spans="1:7" ht="33.5" customHeight="1" thickBot="1">
-      <c r="A22" s="29" t="s">
-        <v>114</v>
-      </c>
-      <c r="B22" s="30" t="e">
-        <f>(0.4*(B20*B20))/B21</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C22" s="21"/>
-      <c r="D22" s="31"/>
-      <c r="E22" s="32"/>
-      <c r="F22" s="33"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="33"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="E13:G13"/>
-    <mergeCell ref="A12:G12"/>
+  <mergeCells count="2">
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="A2:G2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4014,242 +3655,121 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:A79"/>
+  <dimension ref="A2:A39"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="N36" sqref="N36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I42" sqref="I42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="11.25" customHeight="1"/>
   <sheetData>
-    <row r="1" spans="1:1" ht="10.5" customHeight="1">
-      <c r="A1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" ht="10.5" customHeight="1">
+    <row r="2" spans="1:1" ht="11.25" customHeight="1">
       <c r="A2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="10.5" customHeight="1">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="11.25" customHeight="1">
       <c r="A3" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" ht="6" customHeight="1"/>
-    <row r="5" spans="1:1" ht="10.5" customHeight="1">
-      <c r="A5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" ht="6.75" customHeight="1"/>
-    <row r="7" spans="1:1" ht="10.5" customHeight="1">
-      <c r="A7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" ht="10.5" customHeight="1"/>
-    <row r="9" spans="1:1" ht="10.5" customHeight="1">
-      <c r="A9" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" ht="10.5" customHeight="1"/>
-    <row r="11" spans="1:1" ht="10.5" customHeight="1">
-      <c r="A11" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" ht="10.5" customHeight="1"/>
-    <row r="13" spans="1:1" ht="10.5" customHeight="1">
-      <c r="A13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" ht="10.5" customHeight="1">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="11.25" customHeight="1">
+      <c r="A4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="11.25" customHeight="1">
+      <c r="A6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="11.25" customHeight="1">
+      <c r="A8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" ht="11.25" customHeight="1">
+      <c r="A10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" ht="11.25" customHeight="1">
+      <c r="A12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" ht="11.25" customHeight="1">
       <c r="A14" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" ht="10.5" customHeight="1">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" ht="11.25" customHeight="1">
       <c r="A15" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" ht="10.5" customHeight="1"/>
-    <row r="17" spans="1:1" ht="10.5" customHeight="1">
-      <c r="A17" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" ht="10.5" customHeight="1"/>
-    <row r="19" spans="1:1" ht="10.5" customHeight="1">
-      <c r="A19" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" ht="10.5" customHeight="1"/>
-    <row r="21" spans="1:1" ht="10.5" customHeight="1">
-      <c r="A21" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" ht="10.5" customHeight="1"/>
-    <row r="23" spans="1:1" ht="10.5" customHeight="1">
-      <c r="A23" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" ht="10.5" customHeight="1"/>
-    <row r="25" spans="1:1" ht="10.5" customHeight="1">
-      <c r="A25" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" ht="10.5" customHeight="1"/>
-    <row r="27" spans="1:1" ht="10.5" customHeight="1">
-      <c r="A27" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" ht="10.5" customHeight="1"/>
-    <row r="29" spans="1:1" ht="10.5" customHeight="1">
-      <c r="A29" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" ht="7.5" customHeight="1"/>
-    <row r="31" spans="1:1" ht="5.25" customHeight="1"/>
-    <row r="32" spans="1:1" ht="10.5" customHeight="1">
-      <c r="A32" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" ht="10.5" customHeight="1"/>
-    <row r="34" spans="1:1" ht="10.5" customHeight="1">
-      <c r="A34" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" ht="10.5" customHeight="1"/>
-    <row r="36" spans="1:1" ht="10.5" customHeight="1">
-      <c r="A36" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" ht="10.5" customHeight="1"/>
-    <row r="38" spans="1:1" ht="10.5" customHeight="1">
-      <c r="A38" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" ht="11.25" customHeight="1">
-      <c r="A42" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" ht="11.25" customHeight="1">
-      <c r="A43" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" ht="11.25" customHeight="1">
-      <c r="A44" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" ht="11.25" customHeight="1">
-      <c r="A46" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" ht="11.25" customHeight="1">
-      <c r="A48" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" ht="11.25" customHeight="1">
-      <c r="A50" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" ht="11.25" customHeight="1">
-      <c r="A52" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" ht="11.25" customHeight="1">
-      <c r="A54" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" ht="11.25" customHeight="1">
-      <c r="A55" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" ht="11.25" customHeight="1">
-      <c r="A56" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" ht="11.25" customHeight="1">
-      <c r="A58" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" ht="11.25" customHeight="1">
-      <c r="A60" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1" ht="11.25" customHeight="1">
-      <c r="A62" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1" ht="11.25" customHeight="1">
-      <c r="A64" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1" ht="11.25" customHeight="1">
-      <c r="A66" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1" ht="11.25" customHeight="1">
-      <c r="A68" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="70" spans="1:1" ht="11.25" customHeight="1">
-      <c r="A70" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="73" spans="1:1" ht="11.25" customHeight="1">
-      <c r="A73" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="75" spans="1:1" ht="11.25" customHeight="1">
-      <c r="A75" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="77" spans="1:1" ht="11.25" customHeight="1">
-      <c r="A77" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="79" spans="1:1" ht="11.25" customHeight="1">
-      <c r="A79" t="s">
-        <v>101</v>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" ht="11.25" customHeight="1">
+      <c r="A16" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="11.25" customHeight="1">
+      <c r="A18" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" ht="11.25" customHeight="1">
+      <c r="A20" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" ht="11.25" customHeight="1">
+      <c r="A22" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" ht="11.25" customHeight="1">
+      <c r="A24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" ht="11.25" customHeight="1">
+      <c r="A26" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" ht="11.25" customHeight="1">
+      <c r="A28" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" ht="11.25" customHeight="1">
+      <c r="A30" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" ht="11.25" customHeight="1">
+      <c r="A33" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" ht="11.25" customHeight="1">
+      <c r="A35" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" ht="11.25" customHeight="1">
+      <c r="A37" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" ht="11.25" customHeight="1">
+      <c r="A39" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>